<commit_message>
Added the ability to replace with regular expressions
</commit_message>
<xml_diff>
--- a/databank_englishB-copy.xlsx
+++ b/databank_englishB-copy.xlsx
@@ -350,7 +350,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>men / twelve / committee / and / be / the / . / woman / on / there / nine</t>
+          <t>woman / and / men / . / the / be / nine / there / on / twelve / committee</t>
         </is>
       </c>
       <c r="E1" s="1" t="n">
@@ -368,12 +368,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>We don’t have much money now.</t>
+          <t>We don't have much money now.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>. / don / now / ’ / much / t / we / have / money</t>
+          <t>have / money / now / we / . / much / not / do</t>
         </is>
       </c>
       <c r="E2" s="1" t="n">
@@ -396,7 +396,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>have / of / two / paper / can / I / sheets / ?</t>
+          <t>sheets / of / paper / ? / have / I / can / two</t>
         </is>
       </c>
       <c r="E3" s="1" t="n">
@@ -419,7 +419,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>mountain / . / be / the / on / there / many / sheep</t>
+          <t>. / mountain / the / many / be / on / there / sheep</t>
         </is>
       </c>
       <c r="E4" s="1" t="n">
@@ -437,12 +437,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>You can’t enter this building with dangerous things such as knife.</t>
+          <t>You can't enter this building with dangerous things such as knife.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>such / building / . / ’ / things / knife / with / can / as / t / enter / you / this / dangerous</t>
+          <t>enter / can / with / as / . / dangerous / things / knife / this / not / you / such / building</t>
         </is>
       </c>
       <c r="E5" s="1" t="n">
@@ -465,7 +465,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>several / grasses / . / juice / of / drink / we</t>
+          <t>of / juice / . / grasses / drink / we / several</t>
         </is>
       </c>
       <c r="E6" s="1" t="n">
@@ -488,7 +488,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>? / slices / like / of / you / how / bread / would / many</t>
+          <t>slices / ? / bread / would / how / like / you / many / of</t>
         </is>
       </c>
       <c r="E7" s="1" t="n">
@@ -511,7 +511,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>make / taste / your / corn / will / some / better / . / salad</t>
+          <t>your / will / better / corn / taste / salad / . / some / make</t>
         </is>
       </c>
       <c r="E8" s="1" t="n">
@@ -534,7 +534,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>some / I / from / get / Information / the / website / useful / .</t>
+          <t>get / the / from / some / I / website / . / useful / information</t>
         </is>
       </c>
       <c r="E9" s="1" t="n">
@@ -557,7 +557,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>the / some / fish / in / swim / be / . / tank</t>
+          <t>be / . / swim / fish / tank / some / in / the</t>
         </is>
       </c>
       <c r="E10" s="1" t="n">
@@ -580,7 +580,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>. / in / the / refrigerator / be / bottles / milk / two / of / there</t>
+          <t>. / in / milk / of / the / two / there / refrigerator / be / bottles</t>
         </is>
       </c>
       <c r="E11" s="1" t="n">
@@ -603,7 +603,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>much / money / ? / how / do / you / need</t>
+          <t>money / how / much / do / ? / need / you</t>
         </is>
       </c>
       <c r="E12" s="1" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>give / advice / of / a / me / he / this / good / . / piece</t>
+          <t>piece / this / good / of / advice / a / . / he / give / me</t>
         </is>
       </c>
       <c r="E13" s="1" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>author / the / of / he / . / book / this / be</t>
+          <t>he / the / book / this / of / be / author / .</t>
         </is>
       </c>
       <c r="E14" s="1" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>five / the / we / dog / member / . / be / small / a / years / now / . / buy / And / our / ago / dog / a / of / , / family</t>
+          <t>dog / a / ago / dog / of / our / . / buy / member / we / a / now / small / years / , / five / . / and / be / family / the</t>
         </is>
       </c>
       <c r="E15" s="1" t="n">
@@ -695,7 +695,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>in / U.S / the / history / . / study / he / be</t>
+          <t>he / be / in / U.S / . / study / history / the</t>
         </is>
       </c>
       <c r="E16" s="1" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>on / . / the / . / There / snow / ground / watch / step / your / be</t>
+          <t>snow / there / watch / the / . / on / ground / step / be / . / your</t>
         </is>
       </c>
       <c r="E17" s="1" t="n">
@@ -741,7 +741,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>a / to / some / I / Steve / want / . / be / Jobs / day</t>
+          <t>want / Steve / . / be / a / day / I / Jobs / some / to</t>
         </is>
       </c>
       <c r="E18" s="1" t="n">
@@ -764,7 +764,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>a / play / tennis / week / my / twice / father / .</t>
+          <t>tennis / father / week / play / a / my / twice / .</t>
         </is>
       </c>
       <c r="E19" s="1" t="n">
@@ -787,7 +787,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>sell / by / the / be / usually / cream / . / pint / ice</t>
+          <t>sell / cream / pint / be / the / Ice / usually / by / .</t>
         </is>
       </c>
       <c r="E20" s="1" t="n">
@@ -810,7 +810,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>be / father / . / teacher / writer / a / and / his</t>
+          <t>be / his / teacher / and / father / . / writer / a</t>
         </is>
       </c>
       <c r="E21" s="1" t="n">
@@ -833,7 +833,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>buy / a / a / pink / me / white / please / rise / . / and</t>
+          <t>white / pink / me / buy / a / rise / a / please / and / .</t>
         </is>
       </c>
       <c r="E22" s="1" t="n">
@@ -856,7 +856,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>year / at / least / we / meet / to / promise / a / once / a / . / make</t>
+          <t>once / meet / year / at / make / least / we / to / . / a / promise / a</t>
         </is>
       </c>
       <c r="E23" s="1" t="n">
@@ -879,7 +879,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>it / in / make / he / the / sugar / lot / a / cake / of / have / .</t>
+          <t>he / . / have / the / make / of / in / a / it / sugar / lot / cake</t>
         </is>
       </c>
       <c r="E24" s="1" t="n">
@@ -902,7 +902,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ate / of / the / . / slices / ham / boy / two</t>
+          <t>ham / slices / ate / boy / the / . / two / of</t>
         </is>
       </c>
       <c r="E25" s="1" t="n">
@@ -925,7 +925,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>end / all / to / . / good / come / an / things</t>
+          <t>. / good / things / all / an / end / come / to</t>
         </is>
       </c>
       <c r="E26" s="1" t="n">
@@ -948,7 +948,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>. / Kitakami / River / the / town / through / flow / the</t>
+          <t>flow / Kitakami / town / River / . / the / through / the</t>
         </is>
       </c>
       <c r="E27" s="1" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>she / small / a / be / . / baggage / of / piece / carry</t>
+          <t>carry / small / a / she / be / piece / of / baggage / .</t>
         </is>
       </c>
       <c r="E28" s="1" t="n">
@@ -994,7 +994,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>girl / too / be / . / the / jacket / big / wear / a</t>
+          <t>big / be / a / girl / too / jacket / the / wear / .</t>
         </is>
       </c>
       <c r="E29" s="1" t="n">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>be / the / the / half / tomato / . / this / size / I / tomatoes / grow / of</t>
+          <t>be / grow / of / size / . / the / tomato / tomatoes / I / this / half / the</t>
         </is>
       </c>
       <c r="E30" s="1" t="n">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>attract / a / actor / dancer / quite / . / and / large / audience / the</t>
+          <t>and / dancer / attract / a / audience / . / quite / actor / large / the</t>
         </is>
       </c>
       <c r="E31" s="1" t="n">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>a / be / in / . / people / few / restaurant / the / there</t>
+          <t>restaurant / the / . / a / few / be / in / people / there</t>
         </is>
       </c>
       <c r="E32" s="1" t="n">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>game / become / . / crowd / the / excite / when / the / begin</t>
+          <t>begin / crowd / become / the / excite / when / . / game / the</t>
         </is>
       </c>
       <c r="E33" s="1" t="n">
@@ -1104,12 +1104,12 @@
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>I can’t stop reading this book. It’s so interesting.</t>
+          <t>I can't stop reading this book. It's so interesting.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>It / . / interesting / this / . / can / ’ / s / so / t / book / stop / ’ / I / reading</t>
+          <t>so / I / . / it / interesting / be / not / . / book / stop / can / this / reading</t>
         </is>
       </c>
       <c r="E34" s="1" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>sisters / ? / have / do / or / you / any / brothers</t>
+          <t>have / brothers / sisters / or / do / you / ? / any</t>
         </is>
       </c>
       <c r="E35" s="1" t="n">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>expensive / an / , / he / so / little / buy / . / have / he / money / bicycle / now</t>
+          <t>so / , / he / little / . / buy / he / expensive / bicycle / now / have / money / an</t>
         </is>
       </c>
       <c r="E36" s="1" t="n">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>miraculously / . / recover / the / die / whale</t>
+          <t>die / miraculously / . / the / recover / whale</t>
         </is>
       </c>
       <c r="E37" s="1" t="n">
@@ -1196,12 +1196,12 @@
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>I’m looking for a dress similar to yours.</t>
+          <t>I'm looking for a dress similar to yours.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>yours / a / ’ / to / dress / similar / m / . / for / I / look</t>
+          <t>to / similar / yours / I / look / . / a / dress / be / for</t>
         </is>
       </c>
       <c r="E38" s="1" t="n">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>a / girl / . / be / happy / she</t>
+          <t>. / she / a / girl / happy / be</t>
         </is>
       </c>
       <c r="E39" s="1" t="n">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>people / to / some / speech / bored / his / . / fall / during / a / sleep / begin</t>
+          <t>to / fall / a / people / some / during / bored / sleep / . / his / speech / begin</t>
         </is>
       </c>
       <c r="E40" s="1" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>not / better / so / . / cake / you / eat / much / have</t>
+          <t>so / not / better / much / have / . / cake / eat / you</t>
         </is>
       </c>
       <c r="E41" s="1" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>climber / be / . / alive / be / really / lucky / found / the / it</t>
+          <t>it / be / found / really / lucky / alive / the / . / climber / be</t>
         </is>
       </c>
       <c r="E42" s="1" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>hours / medicine / the / take / effect / in / . / few / a / will</t>
+          <t>hours / the / effect / in / . / medicine / a / take / few / will</t>
         </is>
       </c>
       <c r="E43" s="1" t="n">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>he / does / have / children / any / ?</t>
+          <t>he / children / any / ? / have / does</t>
         </is>
       </c>
       <c r="E44" s="1" t="n">
@@ -1357,12 +1357,12 @@
       </c>
       <c r="C45" s="1" t="inlineStr">
         <is>
-          <t>“No, I usually get up quite late.”</t>
+          <t>No, I usually get up quite late.</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>usually / No / late / I / ” / , / get / “ / . / up / quite</t>
+          <t>, / I / get / quite / . / usually / no / up / late</t>
         </is>
       </c>
       <c r="E45" s="1" t="n">
@@ -1380,12 +1380,12 @@
       </c>
       <c r="C46" s="1" t="inlineStr">
         <is>
-          <t>“How often do you go skiing in every winter?”</t>
+          <t>How often do you go skiing in every winter?</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>you / often / winter / ? / in / How / “ / ” / ski / go / every / do</t>
+          <t>ski / do / every / often / go / ? / how / winter / in / you</t>
         </is>
       </c>
       <c r="E46" s="1" t="n">
@@ -1403,12 +1403,12 @@
       </c>
       <c r="C47" s="1" t="inlineStr">
         <is>
-          <t>“Neither could I. We have to work hard tonight.”</t>
+          <t>Neither could I. We have to work hard tonight.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>have / . / We / hard / I / could / to / . / ” / work / Neither / tonight / “</t>
+          <t>neither / . / . / we / work / could / have / I / tonight / to / hard</t>
         </is>
       </c>
       <c r="E47" s="1" t="n">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="C48" s="1" t="inlineStr">
         <is>
-          <t>“So is my sister. The flu is going around.”</t>
+          <t>So is my sister. The flu is going around.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>So / . / sister / flu / be / The / go / my / ” / be / around / . / “</t>
+          <t>go / be / . / the / . / my / around / flu / so / sister / be</t>
         </is>
       </c>
       <c r="E48" s="1" t="n">
@@ -1449,12 +1449,12 @@
       </c>
       <c r="C49" s="1" t="inlineStr">
         <is>
-          <t>“No, she never cooks.”</t>
+          <t>No, she never cooks.</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>, / cook / “ / No / ” / she / never / .</t>
+          <t>, / never / . / cook / no / she</t>
         </is>
       </c>
       <c r="E49" s="1" t="n">
@@ -1472,12 +1472,12 @@
       </c>
       <c r="C50" s="1" t="inlineStr">
         <is>
-          <t>“Don’t rush me. Eating slowly is healthier than eating quickly.”</t>
+          <t>Don't rush me. Eating slowly is healthier than eating quickly.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>” / healthier / me / slowly / than / quickly / . / be / eat / t / “ / Don / rush / ’ / Eating / .</t>
+          <t>eat / rush / . / healthier / do / slowly / quickly / . / not / be / than / eating / me</t>
         </is>
       </c>
       <c r="E50" s="1" t="n">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>woman / . / live / life / happy / the / a</t>
+          <t>a / woman / life / live / the / . / happy</t>
         </is>
       </c>
       <c r="E51" s="1" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>in / man / that / the / office / . / work / hard</t>
+          <t>hard / office / . / in / the / work / that / man</t>
         </is>
       </c>
       <c r="E52" s="1" t="n">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>very / the / uncle / well / my / guitar / . / play</t>
+          <t>very / play / guitar / my / well / the / . / uncle</t>
         </is>
       </c>
       <c r="E53" s="1" t="n">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>saw / he / his / . / way / be / on / it / that / a / bear / surprise / home</t>
+          <t>saw / be / . / home / he / surprise / way / that / it / on / his / bear / a</t>
         </is>
       </c>
       <c r="E54" s="1" t="n">
@@ -1587,12 +1587,12 @@
       </c>
       <c r="C55" s="1" t="inlineStr">
         <is>
-          <t>My friend didn’t have the courage to talk to the famous actor, and I didn’t, either.</t>
+          <t>My friend didn't have the courage to talk to the famous actor, and I didn't, either.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>and / to / have / didn / talk / t / ’ / friend / either / t / didn / famous / to / , / I / courage / actor / , / the / . / the / ’ / my</t>
+          <t>either / courage / talk / do / not / my / to / do / and / friend / the / , / actor / to / the / famous / I / , / not / have / .</t>
         </is>
       </c>
       <c r="E55" s="1" t="n">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>see / enter / to / his / theater / the / movie / professor / the / be / . / often / by / students</t>
+          <t>professor / students / . / enter / to / see / often / his / the / theater / be / by / the / movie</t>
         </is>
       </c>
       <c r="E56" s="1" t="n">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>far / city / the / the / live / away / big / man / . / alone / from</t>
+          <t>big / man / alone / far / away / . / the / live / city / the / from</t>
         </is>
       </c>
       <c r="E57" s="1" t="n">
@@ -1656,12 +1656,12 @@
       </c>
       <c r="C58" s="1" t="inlineStr">
         <is>
-          <t>I don’t eat much meat but I eat a lot of vegetable.</t>
+          <t>I don't eat much meat but I eat a lot of vegetable.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>t / don / I / I / of / . / meat / a / eat / but / eat / ’ / vegetable / much / lot</t>
+          <t>I / eat / meat / lot / much / but / do / not / I / of / vegetable / eat / . / a</t>
         </is>
       </c>
       <c r="E58" s="1" t="n">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>luckily / available / tickets / concert / still / the / . / be / ,</t>
+          <t>luckily / concert / . / still / tickets / available / be / the / ,</t>
         </is>
       </c>
       <c r="E59" s="1" t="n">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>. / sorry / never / to / be / write / I / I / you / really</t>
+          <t>write / I / never / I / you / to / really / . / be / sorry</t>
         </is>
       </c>
       <c r="E60" s="1" t="n">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>hospital / visit / in / sister / . / sometimes / his / only / the / him</t>
+          <t>him / sometimes / sister / visit / only / hospital / his / the / in / .</t>
         </is>
       </c>
       <c r="E61" s="1" t="n">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>apparently / with / . / be / the / something / car / very / , / wrong</t>
+          <t>apparently / car / very / . / the / something / , / wrong / with / be</t>
         </is>
       </c>
       <c r="E62" s="1" t="n">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>miss / the / walk / . / home / and / have / , / he / last / train / unfortunately / to</t>
+          <t>, / home / unfortunately / to / and / have / walk / train / miss / . / last / the / he</t>
         </is>
       </c>
       <c r="E63" s="1" t="n">
@@ -1794,12 +1794,12 @@
       </c>
       <c r="C64" s="1" t="inlineStr">
         <is>
-          <t>I don’t have much knowledge of the subject.</t>
+          <t>I don't have much knowledge of the subject.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>much / I / of / the / ’ / subject / don / t / have / . / knowledge</t>
+          <t>have / do / I / not / . / much / knowledge / the / subject / of</t>
         </is>
       </c>
       <c r="E64" s="1" t="n">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>or / green / , / orange / gloves / be / your / the / , / ones / ones / which / the / ?</t>
+          <t>green / orange / gloves / ones / be / ? / , / ones / or / your / the / which / , / the</t>
         </is>
       </c>
       <c r="E65" s="1" t="n">
@@ -1840,12 +1840,12 @@
       </c>
       <c r="C66" s="1" t="inlineStr">
         <is>
-          <t>I want a new bicycle, but my father won’t buy me one.</t>
+          <t>I want a new bicycle, but my father won't buy me one.</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>’ / . / a / bicycle / but / new / me / one / my / want / t / buy / win / I / father / ,</t>
+          <t>one / father / not / me / buy / I / my / new / want / bicycle / . / will / a / , / but</t>
         </is>
       </c>
       <c r="E66" s="1" t="n">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>all / and / to / down / the / other / sit / . / talk / to / each / begin / students</t>
+          <t>all / . / down / students / to / to / other / and / each / begin / sit / talk / the</t>
         </is>
       </c>
       <c r="E67" s="1" t="n">
@@ -1886,12 +1886,12 @@
       </c>
       <c r="C68" s="1" t="inlineStr">
         <is>
-          <t>I didn’t know where to go or what to do.</t>
+          <t>I didn't know where to go or what to do.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>’ / or / . / didn / go / where / what / t / to / know / to / I / do</t>
+          <t>to / go / or / where / to / do / I / know / . / what / not / do</t>
         </is>
       </c>
       <c r="E68" s="1" t="n">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>across / friend / and / have / , / together / an / they / run / tea / . / some / she / old</t>
+          <t>they / and / old / some / friend / . / run / have / across / she / , / together / tea / an</t>
         </is>
       </c>
       <c r="E69" s="1" t="n">
@@ -1937,7 +1937,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>and / . / speak / slowly / the / they / to / clearly / ask / man</t>
+          <t>man / slowly / . / ask / to / the / speak / they / clearly / and</t>
         </is>
       </c>
       <c r="E70" s="1" t="n">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>cat / scratch / it / , / stop / the / will / or / you / . / bother</t>
+          <t>cat / or / you / bother / . / stop / scratch / the / it / will / ,</t>
         </is>
       </c>
       <c r="E71" s="1" t="n">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>soon / she / did / be / say / that / home / ? / come / she</t>
+          <t>did / that / come / home / be / she / soon / she / say / ?</t>
         </is>
       </c>
       <c r="E72" s="1" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>make / the / to / whether / go / we / be / hold / . / tomorrow / or / be / sure / must / not / meeting</t>
+          <t>to / must / we / meeting / tomorrow / go / not / or / whether / . / be / make / sure / the / be / hold</t>
         </is>
       </c>
       <c r="E73" s="1" t="n">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>whether / ? / know / game / do / win / you / he / the</t>
+          <t>win / know / he / ? / do / game / you / the / whether</t>
         </is>
       </c>
       <c r="E74" s="1" t="n">
@@ -2047,12 +2047,12 @@
       </c>
       <c r="C75" s="1" t="inlineStr">
         <is>
-          <t>I don’t doubt that Mary will be happy to hear the news.</t>
+          <t>I don't doubt that Mary will be happy to hear the news.</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>I / doubt / to / t / that / happy / will / ’ / don / the / hear / news / Mary / be / .</t>
+          <t>will / doubt / do / . / news / happy / the / I / be / Mary / not / hear / that / to</t>
         </is>
       </c>
       <c r="E75" s="1" t="n">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>agree / big / be / not / a / Mr.Tanaka / problem / or / whether / .</t>
+          <t>agree / Mr.Tanaka / not / big / or / be / a / problem / whether / .</t>
         </is>
       </c>
       <c r="E76" s="1" t="n">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>sick / . / worried / look / her / be / she / friend / because / very</t>
+          <t>friend / look / very / she / worried / her / because / sick / . / be</t>
         </is>
       </c>
       <c r="E77" s="1" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>私はお店に買い物をしてる間に財布を無くしました。</t>
+          <t>私はお店に買い物をしている間に財布を無くしました。</t>
         </is>
       </c>
       <c r="C78" s="1" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>I / in / shop / I / . / store / wallet / the / my / while / be / lose</t>
+          <t>shop / while / store / . / my / I / in / the / wallet / lose / I / be</t>
         </is>
       </c>
       <c r="E78" s="1" t="n">
@@ -2139,12 +2139,12 @@
       </c>
       <c r="C79" s="1" t="inlineStr">
         <is>
-          <t>Didn’t you wash your hands before you ate lunch?</t>
+          <t>Didn't you wash your hands before you ate lunch?</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>you / ’ / before / lunch / you / eat / hands / wash / ? / didn / t / your</t>
+          <t>lunch / your / before / not / ? / you / wash / did / hands / eat / you</t>
         </is>
       </c>
       <c r="E79" s="1" t="n">
@@ -2162,12 +2162,12 @@
       </c>
       <c r="C80" s="1" t="inlineStr">
         <is>
-          <t>You can’t use this facility unless you live in this city.</t>
+          <t>You can't use this facility unless you live in this city.</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>facility / use / . / unless / t / live / can / this / ’ / you / you / city / in / this</t>
+          <t>can / live / this / city / unless / not / facility / you / this / . / you / in / use</t>
         </is>
       </c>
       <c r="E80" s="1" t="n">
@@ -2185,12 +2185,12 @@
       </c>
       <c r="C81" s="1" t="inlineStr">
         <is>
-          <t>Let’s go swimming if it isn’t rainy tomorrow.</t>
+          <t>Let's go swimming if it isn't rainy tomorrow.</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>s / rainy / ’ / tomorrow / it / go / isn / let / if / . / t / ’ / swim</t>
+          <t>. / if / go / rainy / be / it / tomorrow / n't / as / swim / let</t>
         </is>
       </c>
       <c r="E81" s="1" t="n">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>for / time / arrive / dinner / so / that / . / hurry / in / we / could / home / we</t>
+          <t>that / for / home / hurry / we / arrive / in / . / we / dinner / could / so / time</t>
         </is>
       </c>
       <c r="E82" s="1" t="n">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>many / but / animals / also / endanger / be / not / only / plants / .</t>
+          <t>plants / also / endanger / animals / . / many / not / only / be / but</t>
         </is>
       </c>
       <c r="E83" s="1" t="n">
@@ -2254,12 +2254,12 @@
       </c>
       <c r="C84" s="1" t="inlineStr">
         <is>
-          <t>The doll house was so delicate that we couldn’t touch it.</t>
+          <t>The doll house was so delicate that we couldn't touch it.</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>doll / be / the / it / ’ / we / couldn / so / that / t / house / touch / delicate / .</t>
+          <t>touch / that / it / we / delicate / the / house / be / could / . / n't / doll / so</t>
         </is>
       </c>
       <c r="E84" s="1" t="n">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>tonight / not / father / be / but / dinner / mother / make / my / . / my</t>
+          <t>tonight / but / . / father / make / my / be / mother / my / dinner / not</t>
         </is>
       </c>
       <c r="E85" s="1" t="n">
@@ -2300,12 +2300,12 @@
       </c>
       <c r="C86" s="1" t="inlineStr">
         <is>
-          <t>Don’t make a sound, or you will wake up that dog.</t>
+          <t>Don't make a sound, or you will wake up that dog.</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>dog / . / you / , / that / or / a / up / ’ / don / make / wake / will / sound / t</t>
+          <t>wake / dog / . / , / that / you / up / will / do / a / sound / or / make / not</t>
         </is>
       </c>
       <c r="E86" s="1" t="n">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>, / sound / a / will / up / you / if / you / dog / that / make / wake / .</t>
+          <t>up / will / a / dog / . / sound / you / make / you / that / , / wake / if</t>
         </is>
       </c>
       <c r="E87" s="1" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>. / behalf / the / to / but / Ken / want / on / a / also / only / Mike / make / not / speech / of / class</t>
+          <t>Ken / want / only / . / of / not / Mike / on / but / the / behalf / to / make / also / speech / class / a</t>
         </is>
       </c>
       <c r="E88" s="1" t="n">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>of / make / as / a / . / Mike / on / as / Ken / behalf / class / want / to / speech / well / the</t>
+          <t>behalf / want / as / Ken / make / the / class / mike / of / on / . / to / speech / as / a / well</t>
         </is>
       </c>
       <c r="E89" s="1" t="n">
@@ -2390,12 +2390,12 @@
       </c>
       <c r="C90" s="1" t="inlineStr">
         <is>
-          <t>I won’t tell it to you if you don’t promise to keep it a secret.</t>
+          <t>I won't tell it to you if you don't promise to keep it a secret.</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>to / t / tell / win / secret / you / t / if / promise / it / don / ’ / I / it / ’ / you / . / a / to / keep</t>
+          <t>not / will / do / tell / keep / if / not / a / you / promise / you / . / it / to / secret / to / it / I</t>
         </is>
       </c>
       <c r="E90" s="1" t="n">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>high / to / me / . / bulbs / ceiling / the / light / the / too / change / for / be</t>
+          <t>bulbs / the / too / me / be / the / to / light / for / high / change / ceiling / .</t>
         </is>
       </c>
       <c r="E91" s="1" t="n">
@@ -2436,12 +2436,12 @@
       </c>
       <c r="C92" s="1" t="inlineStr">
         <is>
-          <t>The ceiling was so high that I couldn’t change the light bulbs.</t>
+          <t>The ceiling was so high that I couldn't change the light bulbs.</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>the / the / couldn / high / ceiling / that / . / change / ’ / t / be / so / light / bulbs / I</t>
+          <t>be / that / high / the / the / could / ceiling / n't / . / change / bulbs / so / light / I</t>
         </is>
       </c>
       <c r="E92" s="1" t="n">
@@ -2459,12 +2459,12 @@
       </c>
       <c r="C93" s="1" t="inlineStr">
         <is>
-          <t>Get on this train, or you won’t get there by noon.</t>
+          <t>Get on this train, or you won't get there by noon.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>’ / there / win / , / train / you / on / or / get / by / t / this / noon / get / .</t>
+          <t>not / noon / . / get / this / or / get / , / you / will / there / on / train / by</t>
         </is>
       </c>
       <c r="E93" s="1" t="n">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>by / on / , / get / . / train / and / will / you / there / this / noon / get</t>
+          <t>you / will / on / there / get / this / by / get / noon / , / . / train / and</t>
         </is>
       </c>
       <c r="E94" s="1" t="n">
@@ -2505,12 +2505,12 @@
       </c>
       <c r="C95" s="1" t="inlineStr">
         <is>
-          <t>You should watch tonight’s game even if you aren’t interested in soccer.</t>
+          <t>You should watch tonight's game even if you aren't interested in soccer.</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>in / tonight / if / aren / you / ’ / game / t / watch / should / even / interested / . / s / you / ’ / soccer</t>
+          <t>. / interested / game / tonight / not / even / you / if / you / be / should / soccer / watch / in / 's</t>
         </is>
       </c>
       <c r="E95" s="1" t="n">
@@ -2528,12 +2528,12 @@
       </c>
       <c r="C96" s="1" t="inlineStr">
         <is>
-          <t>This curry is so hot that I can’t eat all of it.</t>
+          <t>This curry is so hot that I can't eat all of it.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>t / it / I / all / so / this / ’ / eat / . / that / of / can / hot / curry / be</t>
+          <t>curry / I / all / can / not / this / of / . / it / that / be / eat / hot / so</t>
         </is>
       </c>
       <c r="E96" s="1" t="n">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>. / they / to / as / be / be / everybody / accept / want</t>
+          <t>be / everybody / accept / as / they / be / want / to / .</t>
         </is>
       </c>
       <c r="E97" s="1" t="n">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>. / Sapporo / for / leave / on / August / 10th / my / brother</t>
+          <t>leave / brother / . / for / Sapporo / August / on / my / 10th</t>
         </is>
       </c>
       <c r="E98" s="1" t="n">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>clouds / . / over / plane / seem / fly / the / be / the / to</t>
+          <t>the / seem / over / . / to / clouds / fly / the / be / plane</t>
         </is>
       </c>
       <c r="E99" s="1" t="n">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>the / a / among / secret / . / five / of / that / us / be</t>
+          <t>secret / . / of / the / be / a / us / five / that / among</t>
         </is>
       </c>
       <c r="E100" s="1" t="n">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>after / ? / to / you / do / have / do / the / concert / anything</t>
+          <t>concert / ? / do / anything / you / do / to / after / have / the</t>
         </is>
       </c>
       <c r="E101" s="1" t="n">
@@ -2666,12 +2666,12 @@
       </c>
       <c r="C102" s="1" t="inlineStr">
         <is>
-          <t>Let’s meet at the station.</t>
+          <t>Let's meet at the station.</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>let / ’ / the / . / at / station / s / meet</t>
+          <t>station / as / meet / let / . / at / the</t>
         </is>
       </c>
       <c r="E102" s="1" t="n">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>swim / hard / be / to / . / against / stream / it / the</t>
+          <t>stream / against / swim / be / hard / . / it / to / the</t>
         </is>
       </c>
       <c r="E103" s="1" t="n">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>between / girl / . / her / be / the / parents / sit / little</t>
+          <t>sit / between / parents / . / little / her / the / be / girl</t>
         </is>
       </c>
       <c r="E104" s="1" t="n">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>school / . / o / get / day / except / I / Sunday / every</t>
+          <t>o / get / day / Sunday / . / except / every / school / I</t>
         </is>
       </c>
       <c r="E105" s="1" t="n">
@@ -2758,12 +2758,12 @@
       </c>
       <c r="C106" s="1" t="inlineStr">
         <is>
-          <t>It’s a nice day Let’s walk through the park.</t>
+          <t>It's a nice day. Let's walk through the park.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>’ / a / walk / nice / . / Let / through / s / park / ’ / it / day / the / s</t>
+          <t>the / it / day / . / park / through / . / a / be / walk / let / nice / as</t>
         </is>
       </c>
       <c r="E106" s="1" t="n">
@@ -2781,12 +2781,12 @@
       </c>
       <c r="C107" s="1" t="inlineStr">
         <is>
-          <t>I couldn’t see the stage well because there was a tall man sitting in front of me.</t>
+          <t>I couldn't see the stage well because there was a tall man sitting in front of me.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>be / t / . / in / front / tall / there / because / see / stage / I / the / well / a / sit / couldn / ’ / man / me / of</t>
+          <t>be / man / see / sit / . / n't / a / me / could / well / there / stage / of / in / tall / because / front / I / the</t>
         </is>
       </c>
       <c r="E107" s="1" t="n">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>. / you / this / must / finish / the / month / by / this / work / of / end</t>
+          <t>must / work / this / end / this / month / by / . / you / of / the / finish</t>
         </is>
       </c>
       <c r="E108" s="1" t="n">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>will / more / India / about / to / you / trip / tell / me / ? / your</t>
+          <t>tell / will / about / to / trip / India / me / ? / more / you / your</t>
         </is>
       </c>
       <c r="E109" s="1" t="n">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>by / students / school / . / come / to / many / train</t>
+          <t>come / . / train / to / school / by / many / students</t>
         </is>
       </c>
       <c r="E110" s="1" t="n">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>mother / . / makeup / not / her / without / a / mirror / on / put / can / my</t>
+          <t>on / can / put / makeup / without / mother / not / my / . / mirror / a / her</t>
         </is>
       </c>
       <c r="E111" s="1" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>the / . / in / 1915 / world / year / end / War / II</t>
+          <t>War / in / year / World / the / . / II / end / 1915</t>
         </is>
       </c>
       <c r="E112" s="1" t="n">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>people / to / volunteer / . / in / countries / poor / do / want / I / for / work / develop</t>
+          <t>in / poor / want / countries / develop / people / I / to / . / do / volunteer / work / for</t>
         </is>
       </c>
       <c r="E113" s="1" t="n">
@@ -2942,12 +2942,12 @@
       </c>
       <c r="C114" s="1" t="inlineStr">
         <is>
-          <t>My mother’s watch is made in Switzerland.</t>
+          <t>My mother's watch was made in Switzerland.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>watch / in / s / be / Switzerland / mother / ’ / . / my / make</t>
+          <t>Switzerland / in / make / mother / watch / my / be / 's / .</t>
         </is>
       </c>
       <c r="E114" s="1" t="n">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>that / be / what / ? / make / bag / of</t>
+          <t>bag / be / that / make / of / ? / what</t>
         </is>
       </c>
       <c r="E115" s="1" t="n">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>. / make / things / many / be / petroleum / into</t>
+          <t>things / into / . / petroleum / be / make / many</t>
         </is>
       </c>
       <c r="E116" s="1" t="n">
@@ -3011,12 +3011,12 @@
       </c>
       <c r="C117" s="1" t="inlineStr">
         <is>
-          <t>I can’t believe that paper is made from plants.</t>
+          <t>I can't believe that paper is made from plants.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>from / make / I / . / can / be / t / believe / ’ / plants / that / paper</t>
+          <t>plants / make / paper / that / can / . / from / I / be / believe / not</t>
         </is>
       </c>
       <c r="E117" s="1" t="n">
@@ -3034,12 +3034,12 @@
       </c>
       <c r="C118" s="1" t="inlineStr">
         <is>
-          <t>Let’s race to the top of the mountain.</t>
+          <t>Let's race to the top of the mountain.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>to / race / the / mountain / s / . / of / top / ’ / let / the</t>
+          <t>as / to / . / top / let / mountain / the / the / of / race</t>
         </is>
       </c>
       <c r="E118" s="1" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>? / be / cut / to / I / what / go / the / cheese</t>
+          <t>what / I / cheese / the / go / cut / be / to / ?</t>
         </is>
       </c>
       <c r="E119" s="1" t="n">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>. / be / black / women / all / dress / in / of</t>
+          <t>of / women / all / in / dress / be / black / .</t>
         </is>
       </c>
       <c r="E120" s="1" t="n">
@@ -3103,12 +3103,12 @@
       </c>
       <c r="C121" s="1" t="inlineStr">
         <is>
-          <t>We cannot enter the park until nine o’clock.</t>
+          <t>We cannot enter the park until nine o'clock.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>until / park / clock / we / can / . / enter / the / nine / not / ’ / o</t>
+          <t>. / o'clock / park / not / we / enter / until / can / the / nine</t>
         </is>
       </c>
       <c r="E121" s="1" t="n">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>mountains / the / birds / the / fly / over / be / .</t>
+          <t>over / the / mountains / . / the / birds / fly / be</t>
         </is>
       </c>
       <c r="E122" s="1" t="n">
@@ -3149,12 +3149,12 @@
       </c>
       <c r="C123" s="1" t="inlineStr">
         <is>
-          <t>It is raining hard. I don’t want to go out of the building.</t>
+          <t>It is raining hard. I don't want to go out of the building.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>hard / t / . / ’ / it / be / rain / building / want / I / of / go / . / don / out / to / the</t>
+          <t>of / rain / not / it / be / want / building / to / I / do / hard / go / out / . / the / .</t>
         </is>
       </c>
       <c r="E123" s="1" t="n">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>be / their / from / the / look / they / newcomers / at / . / behind / door</t>
+          <t>from / look / door / their / at / behind / . / the / newcomers / they / be</t>
         </is>
       </c>
       <c r="E124" s="1" t="n">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>river / children / and / run / jump / into / the / start / . / the</t>
+          <t>children / jump / the / . / run / start / and / river / the / into</t>
         </is>
       </c>
       <c r="E125" s="1" t="n">
@@ -3218,12 +3218,12 @@
       </c>
       <c r="C126" s="1" t="inlineStr">
         <is>
-          <t>Let’s hope nothing like this will happen again.</t>
+          <t>Let's hope nothing like this will happen again.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>s / will / . / ’ / hope / let / this / again / nothing / like / happen</t>
+          <t>happen / as / let / nothing / again / will / hope / this / . / like</t>
         </is>
       </c>
       <c r="E126" s="1" t="n">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>? / you / do / do / what</t>
+          <t>? / what / do / do / you</t>
         </is>
       </c>
       <c r="E127" s="1" t="n">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>you / or / mineral / water / , / would / like / ? / which / tea</t>
+          <t>or / which / water / tea / mineral / would / ? / , / like / you</t>
         </is>
       </c>
       <c r="E128" s="1" t="n">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>you / work / ? / go / do / how / to</t>
+          <t>how / work / do / to / ? / go / you</t>
         </is>
       </c>
       <c r="E129" s="1" t="n">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>your / when / birthday / ? / be</t>
+          <t>? / when / your / birthday / be</t>
         </is>
       </c>
       <c r="E130" s="1" t="n">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>next / time / the / what / ? / do / come / bus</t>
+          <t>the / ? / time / next / bus / what / do / come</t>
         </is>
       </c>
       <c r="E131" s="1" t="n">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>York / he / stay / long / in / ? / how / do / New</t>
+          <t>? / New / he / in / do / York / long / stay / how</t>
         </is>
       </c>
       <c r="E132" s="1" t="n">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>the / way / do / man / which / ? / go</t>
+          <t>do / the / way / man / which / ? / go</t>
         </is>
       </c>
       <c r="E133" s="1" t="n">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>we / ? / where / now / be</t>
+          <t>? / where / we / now / be</t>
         </is>
       </c>
       <c r="E134" s="1" t="n">
@@ -3425,12 +3425,12 @@
       </c>
       <c r="C135" s="1" t="inlineStr">
         <is>
-          <t>Didn’t you meet Jane at the station?</t>
+          <t>Didn't you meet Jane at the station?</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>the / didn / t / ? / at / Jane / station / meet / ’ / you</t>
+          <t>station / the / not / Jane / did / ? / you / at / meet</t>
         </is>
       </c>
       <c r="E135" s="1" t="n">
@@ -3448,12 +3448,12 @@
       </c>
       <c r="C136" s="1" t="inlineStr">
         <is>
-          <t>He wasn’t born in Japan, was he?</t>
+          <t>He wasn't born in Japan, was he?</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>wasn / in / ? / bear / t / Japan / , / ’ / he / be / he</t>
+          <t>be / he / in / bear / not / Japan / he / , / be / ?</t>
         </is>
       </c>
       <c r="E136" s="1" t="n">
@@ -3471,12 +3471,12 @@
       </c>
       <c r="C137" s="1" t="inlineStr">
         <is>
-          <t>I don’t have much time. How about you?</t>
+          <t>I don't have much time. How about you?</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>I / about / . / you / How / t / have / time / ’ / much / don / ?</t>
+          <t>much / I / time / . / have / you / how / do / ? / about / not</t>
         </is>
       </c>
       <c r="E137" s="1" t="n">
@@ -3499,7 +3499,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>? / what / like / teacher / new / the / math / be</t>
+          <t>teacher / like / new / math / what / be / ? / the</t>
         </is>
       </c>
       <c r="E138" s="1" t="n">
@@ -3517,12 +3517,12 @@
       </c>
       <c r="C139" s="1" t="inlineStr">
         <is>
-          <t>Why don’t you ask her about it on the phone?</t>
+          <t>Why don't you ask her about it on the phone?</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>why / t / don / you / the / about / on / ask / it / her / ? / phone / ’</t>
+          <t>you / her / ask / the / not / ? / do / on / it / about / why / phone</t>
         </is>
       </c>
       <c r="E139" s="1" t="n">
@@ -3540,12 +3540,12 @@
       </c>
       <c r="C140" s="1" t="inlineStr">
         <is>
-          <t>Maki and Dina are good friend aren’t they?</t>
+          <t>Maki and Dina are good friend aren't they?</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>aren / and / t / ’ / Dina / good / maki / they / be / friend / ?</t>
+          <t>good / Dina / ? / they / Maki / not / friend / be / and / be</t>
         </is>
       </c>
       <c r="E140" s="1" t="n">
@@ -3568,7 +3568,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>book / ? / how / the / find / he / do</t>
+          <t>how / book / ? / do / the / find / he</t>
         </is>
       </c>
       <c r="E141" s="1" t="n">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>why / like / this / they / song / ? / do</t>
+          <t>? / song / like / do / they / why / this</t>
         </is>
       </c>
       <c r="E142" s="1" t="n">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>know / I / to / ? / where / make / these / be / baskets / want</t>
+          <t>where / know / be / ? / I / to / these / want / baskets / make</t>
         </is>
       </c>
       <c r="E143" s="1" t="n">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>much / ? / me / tell / how / Yokohama / to / please / the / be / ticket</t>
+          <t>? / how / tell / me / be / ticket / much / Yokohama / please / the / to</t>
         </is>
       </c>
       <c r="E144" s="1" t="n">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>? / what / Dark / color / uniform / . / be / their / green</t>
+          <t>be / dark / what / their / ? / green / uniform / . / color</t>
         </is>
       </c>
       <c r="E145" s="1" t="n">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>museum / the / on / . / ? / to / take / from / foot / About / do / how / minutes / here / it / long / 10</t>
+          <t>long / to / from / about / minutes / take / ? / the / here / . / on / 10 / museum / it / how / foot / do</t>
         </is>
       </c>
       <c r="E146" s="1" t="n">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>problem / be / Nobody / able / to / solve / the / who / ? / .</t>
+          <t>solve / who / be / nobody / ? / . / the / to / problem / able</t>
         </is>
       </c>
       <c r="E147" s="1" t="n">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>about / go / Why / Saturday / ? / next / not / the / to / ? / how / movies</t>
+          <t>next / how / to / ? / why / movies / about / the / ? / go / not / Saturday</t>
         </is>
       </c>
       <c r="E148" s="1" t="n">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>town / move / friend / best / be / another / be / you / My / so / ? / sad / . / why / to</t>
+          <t>why / to / ? / you / town / my / friend / move / sad / another / be / so / be / . / best</t>
         </is>
       </c>
       <c r="E149" s="1" t="n">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>new / what / ? / their / house / like / be</t>
+          <t>like / ? / house / be / what / new / their</t>
         </is>
       </c>
       <c r="E150" s="1" t="n">
@@ -3793,12 +3793,12 @@
       </c>
       <c r="C151" s="1" t="inlineStr">
         <is>
-          <t>Why isn’t Jack playing on this team?</t>
+          <t>Why isn't Jack playing on this team?</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>this / ’ / playing / Jack / on / why / t / isn / ? / team</t>
+          <t>why / ? / be / this / team / Jack / n't / play / on</t>
         </is>
       </c>
       <c r="E151" s="1" t="n">
@@ -3816,12 +3816,12 @@
       </c>
       <c r="C152" s="1" t="inlineStr">
         <is>
-          <t>The meeting does start until 10 o’clock, doesn’t it?</t>
+          <t>The meeting does start until 10 o'clock, doesn't it?</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>10 / start / until / doesn / ’ / , / t / clock / it / meeting / ? / the / ’ / do / o</t>
+          <t>do / 10 / , / it / do / meeting / not / o'clock / until / the / start / ?</t>
         </is>
       </c>
       <c r="E152" s="1" t="n">
@@ -3839,12 +3839,12 @@
       </c>
       <c r="C153" s="1" t="inlineStr">
         <is>
-          <t>Why don’t we invite Bob and Naomi to the barbecue?</t>
+          <t>Why don't we invite Bob and Naomi to the barbecue?</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>don / Bob / the / and / to / t / ? / we / why / Naomi / invite / ’ / barbecue</t>
+          <t>Bob / not / why / barbecue / to / the / and / ? / Naomi / do / invite / we</t>
         </is>
       </c>
       <c r="E153" s="1" t="n">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>for / the / me / hold / will / door / ? / , / you</t>
+          <t>, / you / will / the / for / door / hold / me / ?</t>
         </is>
       </c>
       <c r="E154" s="1" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>think / come / from / where / do / you / he / ?</t>
+          <t>from / think / ? / he / come / do / where / you</t>
         </is>
       </c>
       <c r="E155" s="1" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>the / think / game / would / I / to / he / come / .</t>
+          <t>come / . / game / would / I / think / to / he / the</t>
         </is>
       </c>
       <c r="E156" s="1" t="n">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>know / ? / the / mine / bicycle / you / be / did / that</t>
+          <t>? / know / mine / the / that / bicycle / did / be / you</t>
         </is>
       </c>
       <c r="E157" s="1" t="n">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>we / down / found / that / . / the / out / tree / have / fall</t>
+          <t>out / . / tree / found / down / have / fall / we / the / that</t>
         </is>
       </c>
       <c r="E158" s="1" t="n">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>that / company / he / john / Japanese / for / work / a / say / .</t>
+          <t>work / for / he / say / John / company / a / . / japanese / that</t>
         </is>
       </c>
       <c r="E159" s="1" t="n">
@@ -4005,7 +4005,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>speak / . / say / very / Chinese / well / you / that / you</t>
+          <t>you / speak / chinese / you / . / that / well / very / say</t>
         </is>
       </c>
       <c r="E160" s="1" t="n">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>. / say / would / school / her / her / drive / cindy / brother / that / to</t>
+          <t>would / drive / say / that / school / Cindy / her / . / her / brother / to</t>
         </is>
       </c>
       <c r="E161" s="1" t="n">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>that / really / he / to / always / . / students / be / lucky / teacher / say / good / have / our</t>
+          <t>. / good / be / teacher / that / have / really / to / students / he / lucky / our / always / say</t>
         </is>
       </c>
       <c r="E162" s="1" t="n">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>he / tell / that / mathematics / us / . / teach / us / mr.yasuda / would</t>
+          <t>us / would / that / Mr.Yasuda / he / teach / . / mathematics / tell / us</t>
         </is>
       </c>
       <c r="E163" s="1" t="n">
@@ -4092,12 +4092,12 @@
       </c>
       <c r="C164" s="1" t="inlineStr">
         <is>
-          <t>The boy said to the soccer player, “ I have always wanted to talk to him.”</t>
+          <t>The boy said to the soccer player, " I have always wanted to talk to you."</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>to / to / always / ” / player / “ / the / have / say / boy / to / I / , / . / soccer / him / talk / want / the</t>
+          <t>to / say / boy / to / to / the / have / soccer / , / the / you / I / . / want / player / talk / `` / always / ''</t>
         </is>
       </c>
       <c r="E164" s="1" t="n">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>the / paper / dog / . / the / girl / her / her / bring / news / tell / to</t>
+          <t>the / dog / her / bring / paper / her / tell / news / the / . / girl / to</t>
         </is>
       </c>
       <c r="E165" s="1" t="n">
@@ -4138,12 +4138,12 @@
       </c>
       <c r="C166" s="1" t="inlineStr">
         <is>
-          <t>The tourist said to the conductor, “Please tell me the way to the hotel.”</t>
+          <t>The tourist said to the conductor, "Please tell me the way to the hotel."</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>tourist / conductor / “ / to / to / , / me / Please / hotel / tell / the / say / the / ” / the / way / . / the</t>
+          <t>me / hotel / '' / way / to / tell / the / please / the / conductor / . / tourist / , / `` / the / the / say / to</t>
         </is>
       </c>
       <c r="E166" s="1" t="n">
@@ -4161,12 +4161,12 @@
       </c>
       <c r="C167" s="1" t="inlineStr">
         <is>
-          <t>The old man always says to us “How are you?”</t>
+          <t>The old man always says to us "How are you?"</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>How / you / ” / say / us / ? / man / old / always / to / the / “ / be</t>
+          <t>to / always / us / old / how / man / be / `` / you / ? / the / '' / say</t>
         </is>
       </c>
       <c r="E167" s="1" t="n">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>my / be / have / me / I / where / ask / mother / ?</t>
+          <t>be / have / I / ask / mother / my / ? / where / me</t>
         </is>
       </c>
       <c r="E168" s="1" t="n">
@@ -4212,7 +4212,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>that / the / man / next / say / day / would / delivery / back / the / he / come / .</t>
+          <t>the / man / say / would / come / delivery / . / back / next / he / the / day / that</t>
         </is>
       </c>
       <c r="E169" s="1" t="n">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>teacher / the / that / before / . / a / day / tell / he / the / him / good / have / do / job</t>
+          <t>him / do / day / teacher / the / tell / good / before / . / a / job / the / have / that / he</t>
         </is>
       </c>
       <c r="E170" s="1" t="n">
@@ -4258,7 +4258,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>me / meet / next / ask / her / the / . / the / to / there / woman / morning</t>
+          <t>meet / me / to / her / next / woman / the / . / the / morning / there / ask</t>
         </is>
       </c>
       <c r="E171" s="1" t="n">
@@ -4276,12 +4276,12 @@
       </c>
       <c r="C172" s="1" t="inlineStr">
         <is>
-          <t>The villager asked him why he hadn’t came to work the previous week?</t>
+          <t>The villager asked him why he hadn't came to work the previous week?</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>him / villager / he / the / come / previous / why / ? / ask / ’ / t / work / hadn / week / to / the</t>
+          <t>come / work / the / have / week / him / the / previous / villager / why / ask / ? / n't / to / he</t>
         </is>
       </c>
       <c r="E172" s="1" t="n">
@@ -4299,12 +4299,12 @@
       </c>
       <c r="C173" s="1" t="inlineStr">
         <is>
-          <t>The students said to the woman “We are going to stay at this hotel tonight.</t>
+          <t>The students said to the woman "We are going to stay at this hotel tonight.</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>the / this / to / We / at / students / to / tonight / . / be / stay / go / the / “ / say / woman / hotel</t>
+          <t>we / . / go / `` / say / this / stay / the / to / tonight / woman / students / the / at / hotel / be / to</t>
         </is>
       </c>
       <c r="E173" s="1" t="n">
@@ -4322,12 +4322,12 @@
       </c>
       <c r="C174" s="1" t="inlineStr">
         <is>
-          <t>I didn’t know you were a friend of the famous writer.</t>
+          <t>I didn't know you were a friend of the famous writer.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>writer / famous / t / friend / be / . / I / the / ’ / you / a / of / didn / know</t>
+          <t>the / be / I / . / do / famous / writer / you / know / a / friend / not / of</t>
         </is>
       </c>
       <c r="E174" s="1" t="n">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="C175" s="1" t="inlineStr">
         <is>
-          <t>I didn’t know you were a friend of the famous writer.</t>
+          <t>I didn't know you were a friend of the famous writer.</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>t / ’ / a / writer / be / didn / the / famous / you / know / I / friend / . / of</t>
+          <t>be / of / do / a / not / you / . / famous / friend / the / writer / know / I</t>
         </is>
       </c>
       <c r="E175" s="1" t="n">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>ask / the / if / early / teacher / . / home / could / student / go / the / he</t>
+          <t>the / if / . / go / he / ask / could / early / teacher / student / home / the</t>
         </is>
       </c>
       <c r="E176" s="1" t="n">
@@ -4396,7 +4396,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>he / the / man / arrive / ask / old / when / his / . / grandson</t>
+          <t>ask / his / when / old / the / man / he / . / grandson / arrive</t>
         </is>
       </c>
       <c r="E177" s="1" t="n">
@@ -4419,7 +4419,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>tell / stay / there / police / men / the / officer / . / to / the / young</t>
+          <t>the / to / officer / men / stay / tell / there / young / police / the / .</t>
         </is>
       </c>
       <c r="E178" s="1" t="n">

</xml_diff>